<commit_message>
Agregado informe 2.6, aplicación de CSS, agregado una vista main además de un apartado para registro de usuarios, añadido archivo sql para base de datos y por ultimo la creación del diagrama E-R
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Documentación/Product Backlog.xlsx
+++ b/Fase 2/Evidencias Proyecto/Documentación/Product Backlog.xlsx
@@ -5,13 +5,15 @@
   <sheets>
     <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Hoja 1'!$A$1:$K$40</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="144">
   <si>
     <t>Prioridad</t>
   </si>
@@ -46,7 +48,61 @@
     <t>Observaciones / Sprint</t>
   </si>
   <si>
-    <t>SPRINT 1: INFRAESTRUCTURA Y CATALOGACIÓN CORE (7 ÍTEMS)</t>
+    <t>FASE 0: SPRINT-PLANING (PLANIFICACIÓN Y DEFINICIÓN)</t>
+  </si>
+  <si>
+    <t>T-PRE01</t>
+  </si>
+  <si>
+    <t>Infra/Plan</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Elaboración del Product Backlog completo</t>
+  </si>
+  <si>
+    <t>Medio</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>Backlog aprobado por Product Owner.</t>
+  </si>
+  <si>
+    <t>PRE-SPRINT</t>
+  </si>
+  <si>
+    <t>T-PRE02</t>
+  </si>
+  <si>
+    <t>Planif.</t>
+  </si>
+  <si>
+    <t>Diseño del Modelo Entidad-Relación (E-R)</t>
+  </si>
+  <si>
+    <t>Diagrama E-R validado contra requisitos de Circulación.</t>
+  </si>
+  <si>
+    <t>T-PRE03</t>
+  </si>
+  <si>
+    <t>Redacción de Historias de Usuario (HU) y Criterios de Aceptación (Clave).</t>
+  </si>
+  <si>
+    <t>Bajo</t>
+  </si>
+  <si>
+    <t>100% de la funcionalidad mapeada.</t>
+  </si>
+  <si>
+    <t>SPRINT 1: INFRAESTRUCTURA Y CATALOGACIÓN CORE</t>
   </si>
   <si>
     <t>T01</t>
@@ -55,21 +111,9 @@
     <t>Infra</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>Configuración del entorno (Flask, MySQL, Conectores) y estructura base del proyecto.</t>
   </si>
   <si>
-    <t>Bajo</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>DONE</t>
-  </si>
-  <si>
     <t>Entorno virtual y conexión a BD validados.</t>
   </si>
   <si>
@@ -82,9 +126,6 @@
     <t>Modelo de Datos v2.0: Creación de todas las tablas con FK y ejemplares_disponibles.</t>
   </si>
   <si>
-    <t>Medio</t>
-  </si>
-  <si>
     <t>Todas las FK y la relación N:M operativas.</t>
   </si>
   <si>
@@ -118,219 +159,222 @@
     <t>API y tabla de Listado de materiales (READ) con JOINs a Autor, Editorial y stock.</t>
   </si>
   <si>
+    <t>La tabla muestra nombres completos de Autor/Editorial, no solo IDs.</t>
+  </si>
+  <si>
+    <t>T03</t>
+  </si>
+  <si>
+    <t>CRUD (CREATE, READ, UPDATE, DELETE) para las tablas de apoyo AUTOR/EDITORIAL.</t>
+  </si>
+  <si>
+    <t>Permite al bibliotecario gestionar los catálogos de metadatos.</t>
+  </si>
+  <si>
+    <t>T06</t>
+  </si>
+  <si>
+    <t>Administración</t>
+  </si>
+  <si>
+    <t>Creación y setup de la tabla USUARIOS (para personal y estudiantes).</t>
+  </si>
+  <si>
+    <t>La tabla está lista para ser poblada con credenciales.</t>
+  </si>
+  <si>
+    <t>SPRINT 2: CATALOGACIÓN AVANZADA Y CIRCULACIÓN START</t>
+  </si>
+  <si>
+    <t>HU-CAT04</t>
+  </si>
+  <si>
+    <t>Implementar funcionalidad de Modificar los datos (UPDATE) de un material catalogado.</t>
+  </si>
+  <si>
+    <t>Alto</t>
+  </si>
+  <si>
+    <t>Validación de stock: Nuevo Total &gt;= Disponibles.</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>HU-CAT06</t>
+  </si>
+  <si>
+    <t>Gestión N:M: Asignar/Desasignar múltiples categorías (MATERIALES_CATEGORIAS).</t>
+  </si>
+  <si>
+    <t>Persistencia correcta de la selección en la tabla pivote.</t>
+  </si>
+  <si>
+    <t>HU-CAT05</t>
+  </si>
+  <si>
+    <t>Implementar la funcionalidad de Eliminar un material (DELETE), con validación de préstamos activos.</t>
+  </si>
+  <si>
+    <t>Si hay préstamos activos, el sistema debe bloquear la eliminación.</t>
+  </si>
+  <si>
+    <t>HU-CIRC01</t>
+  </si>
+  <si>
+    <t>Circulación</t>
+  </si>
+  <si>
+    <t>API y UI para Iniciar un Préstamo (validación de stock, registro y decremento de stock).</t>
+  </si>
+  <si>
+    <t>T06, HU-CAT03</t>
+  </si>
+  <si>
+    <t>ejemplares_disponibles decrementa en 1; PRESTAMOS.estado = 'Activo'.</t>
+  </si>
+  <si>
+    <t>HU-CIRC04</t>
+  </si>
+  <si>
+    <t>Módulo de visualización de Préstamos Activos y Vencidos para el Bibliotecario.</t>
+  </si>
+  <si>
+    <t>Lista filtrada y paginada de préstamos no devueltos.</t>
+  </si>
+  <si>
+    <t>SPRINT 3: CIRCULACIÓN CORE Y OPAC START</t>
+  </si>
+  <si>
+    <t>HU-CIRC02</t>
+  </si>
+  <si>
+    <t>API y UI para Marcar un préstamo como devuelto (actualización de PRESTAMOS e incremento de stock).</t>
+  </si>
+  <si>
+    <t>ejemplares_disponibles incrementa en 1; PRESTAMOS.estado = 'Devuelto'.</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>HU-CIRC03</t>
+  </si>
+  <si>
+    <t>Lógica de negocio para Cálculo automático de Multas al registrar una devolución tardía.</t>
+  </si>
+  <si>
+    <t>Cálculo basado en la diferencia entre fecha_devolucion esperada y real.</t>
+  </si>
+  <si>
+    <t>HU-CONS01</t>
+  </si>
+  <si>
+    <t>OPAC</t>
+  </si>
+  <si>
+    <t>Interfaz Pública (Frontend) con Motor de Búsqueda avanzado (por Título, Autor, Categoría).</t>
+  </si>
+  <si>
+    <t>Búsqueda rápida que utiliza índices de BD.</t>
+  </si>
+  <si>
+    <t>HU-CONS02</t>
+  </si>
+  <si>
+    <t>Vista de Detalle del Material que muestra stock disponible, sinopsis y categorías.</t>
+  </si>
+  <si>
+    <t>Muestra el estado "Disponible" solo si ejemplares_disponibles &gt; 0.</t>
+  </si>
+  <si>
+    <t>T07</t>
+  </si>
+  <si>
+    <t>Implementar un sistema de cache básico para las listas de apoyo (Autores/Editoriales) en Flask.</t>
+  </si>
+  <si>
+    <t>Las listas se cargan desde cache en peticiones sucesivas.</t>
+  </si>
+  <si>
+    <t>SPRINT 4: MÓDULO DE ADMINISTRACIÓN CORE Y OPAC FINISH</t>
+  </si>
+  <si>
+    <t>HU-ADMIN01</t>
+  </si>
+  <si>
+    <t>Módulo de Autenticación (Login) seguro con gestión de sesiones.</t>
+  </si>
+  <si>
+    <t>Uso de hashes (bcrypt) para contraseñas; manejo de errores.</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>HU-ADMIN02</t>
+  </si>
+  <si>
+    <t>CRUD para la tabla USUARIOS (Creación, edición y bloqueo de cuentas de personal y estudiantes).</t>
+  </si>
+  <si>
+    <t>Validación de formato RUT y correo electrónico.</t>
+  </si>
+  <si>
+    <t>HU-ADMIN03</t>
+  </si>
+  <si>
+    <t>Implementación de Roles y Permisos (Restricción de acceso a módulos específicos según el rol).</t>
+  </si>
+  <si>
+    <t>Solo el rol 'Admin' puede acceder al CRUD de Usuarios.</t>
+  </si>
+  <si>
+    <t>HU-CONS03</t>
+  </si>
+  <si>
+    <t>Diseño Responsivo y Optimización de la Interfaz OPAC para móvil.</t>
+  </si>
+  <si>
+    <t>Cumplimiento con validadores de layout (ej. CSS Media Queries).</t>
+  </si>
+  <si>
+    <t>HU-ADMIN04</t>
+  </si>
+  <si>
+    <t>Reporte de Uso: Generar un reporte de los 10 materiales más prestados.</t>
+  </si>
+  <si>
+    <t>Exportable a CSV/Excel.</t>
+  </si>
+  <si>
+    <t>HU-ADMIN05</t>
+  </si>
+  <si>
+    <t>Reporte de Mora: Listado de usuarios con préstamos vencidos y multas calculadas.</t>
+  </si>
+  <si>
+    <t>Cálculo final de multas y filtro por morosidad.</t>
+  </si>
+  <si>
+    <t>FASE FINAL: CERTIFICACIÓN, OPTIMIZACIÓN Y CIERRE (Post-Sprints)</t>
+  </si>
+  <si>
+    <t>T08</t>
+  </si>
+  <si>
+    <t>Infraestructura</t>
+  </si>
+  <si>
+    <t>Implementar logging centralizado para errores de Flask y consultas SQL.</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
     <t>TO DO</t>
   </si>
   <si>
-    <t>La tabla muestra nombres completos de Autor/Editorial, no solo IDs.</t>
-  </si>
-  <si>
-    <t>T03</t>
-  </si>
-  <si>
-    <t>CRUD (CREATE, READ, UPDATE, DELETE) para las tablas de apoyo AUTOR/EDITORIAL.</t>
-  </si>
-  <si>
-    <t>Permite al bibliotecario gestionar los catálogos de metadatos.</t>
-  </si>
-  <si>
-    <t>T06</t>
-  </si>
-  <si>
-    <t>Administración</t>
-  </si>
-  <si>
-    <t>Creación y setup de la tabla USUARIOS (para personal y estudiantes).</t>
-  </si>
-  <si>
-    <t>La tabla está lista para ser poblada con credenciales.</t>
-  </si>
-  <si>
-    <t>SPRINT 2: CATALOGACIÓN AVANZADA Y CIRCULACIÓN START</t>
-  </si>
-  <si>
-    <t>HU-CAT04</t>
-  </si>
-  <si>
-    <t>Implementar funcionalidad de Modificar los datos (UPDATE) de un material catalogado.</t>
-  </si>
-  <si>
-    <t>Alto</t>
-  </si>
-  <si>
-    <t>Validación de stock: Nuevo Total &gt;= Disponibles.</t>
-  </si>
-  <si>
-    <t>Sprint 2</t>
-  </si>
-  <si>
-    <t>HU-CAT06</t>
-  </si>
-  <si>
-    <t>Gestión N:M: Asignar/Desasignar múltiples categorías (MATERIALES_CATEGORIAS).</t>
-  </si>
-  <si>
-    <t>Persistencia correcta de la selección en la tabla pivote.</t>
-  </si>
-  <si>
-    <t>HU-CAT05</t>
-  </si>
-  <si>
-    <t>Implementar la funcionalidad de Eliminar un material (DELETE), con validación de préstamos activos.</t>
-  </si>
-  <si>
-    <t>Si hay préstamos activos, el sistema debe bloquear la eliminación.</t>
-  </si>
-  <si>
-    <t>HU-CIRC01</t>
-  </si>
-  <si>
-    <t>Circulación</t>
-  </si>
-  <si>
-    <t>API y UI para Iniciar un Préstamo (validación de stock, registro y decremento de stock).</t>
-  </si>
-  <si>
-    <t>T06, HU-CAT03</t>
-  </si>
-  <si>
-    <t>ejemplares_disponibles decrementa en 1; PRESTAMOS.estado = 'Activo'.</t>
-  </si>
-  <si>
-    <t>HU-CIRC04</t>
-  </si>
-  <si>
-    <t>Módulo de visualización de Préstamos Activos y Vencidos para el Bibliotecario.</t>
-  </si>
-  <si>
-    <t>Lista filtrada y paginada de préstamos no devueltos.</t>
-  </si>
-  <si>
-    <t>SPRINT 3: CIRCULACIÓN CORE Y OPAC START</t>
-  </si>
-  <si>
-    <t>HU-CIRC02</t>
-  </si>
-  <si>
-    <t>API y UI para Marcar un préstamo como devuelto (actualización de PRESTAMOS e incremento de stock).</t>
-  </si>
-  <si>
-    <t>ejemplares_disponibles incrementa en 1; PRESTAMOS.estado = 'Devuelto'.</t>
-  </si>
-  <si>
-    <t>Sprint 3</t>
-  </si>
-  <si>
-    <t>HU-CIRC03</t>
-  </si>
-  <si>
-    <t>Lógica de negocio para Cálculo automático de Multas al registrar una devolución tardía.</t>
-  </si>
-  <si>
-    <t>Cálculo basado en la diferencia entre fecha_devolucion esperada y real.</t>
-  </si>
-  <si>
-    <t>HU-CONS01</t>
-  </si>
-  <si>
-    <t>OPAC</t>
-  </si>
-  <si>
-    <t>Interfaz Pública (Frontend) con Motor de Búsqueda avanzado (por Título, Autor, Categoría).</t>
-  </si>
-  <si>
-    <t>Búsqueda rápida que utiliza índices de BD.</t>
-  </si>
-  <si>
-    <t>HU-CONS02</t>
-  </si>
-  <si>
-    <t>Vista de Detalle del Material que muestra stock disponible, sinopsis y categorías.</t>
-  </si>
-  <si>
-    <t>Muestra el estado "Disponible" solo si ejemplares_disponibles &gt; 0.</t>
-  </si>
-  <si>
-    <t>T07</t>
-  </si>
-  <si>
-    <t>Implementar un sistema de cache básico para las listas de apoyo (Autores/Editoriales) en Flask.</t>
-  </si>
-  <si>
-    <t>Las listas se cargan desde cache en peticiones sucesivas.</t>
-  </si>
-  <si>
-    <t>SPRINT 4: MÓDULO DE ADMINISTRACIÓN CORE Y OPAC FINISH</t>
-  </si>
-  <si>
-    <t>HU-ADMIN01</t>
-  </si>
-  <si>
-    <t>Módulo de Autenticación (Login) seguro con gestión de sesiones.</t>
-  </si>
-  <si>
-    <t>Uso de hashes (bcrypt) para contraseñas; manejo de errores.</t>
-  </si>
-  <si>
-    <t>Sprint 4</t>
-  </si>
-  <si>
-    <t>HU-ADMIN02</t>
-  </si>
-  <si>
-    <t>CRUD para la tabla USUARIOS (Creación, edición y bloqueo de cuentas de personal y estudiantes).</t>
-  </si>
-  <si>
-    <t>Validación de formato RUT y correo electrónico.</t>
-  </si>
-  <si>
-    <t>HU-ADMIN03</t>
-  </si>
-  <si>
-    <t>Implementación de Roles y Permisos (Restricción de acceso a módulos específicos según el rol).</t>
-  </si>
-  <si>
-    <t>Solo el rol 'Admin' puede acceder al CRUD de Usuarios.</t>
-  </si>
-  <si>
-    <t>HU-CONS03</t>
-  </si>
-  <si>
-    <t>Diseño Responsivo y Optimización de la Interfaz OPAC para móvil.</t>
-  </si>
-  <si>
-    <t>Cumplimiento con validadores de layout (ej. CSS Media Queries).</t>
-  </si>
-  <si>
-    <t>HU-ADMIN04</t>
-  </si>
-  <si>
-    <t>Reporte de Uso: Generar un reporte de los 10 materiales más prestados.</t>
-  </si>
-  <si>
-    <t>Exportable a CSV/Excel.</t>
-  </si>
-  <si>
-    <t>HU-ADMIN05</t>
-  </si>
-  <si>
-    <t>Reporte de Mora: Listado de usuarios con préstamos vencidos y multas calculadas.</t>
-  </si>
-  <si>
-    <t>Cálculo final de multas y filtro por morosidad.</t>
-  </si>
-  <si>
-    <t>FASE FINAL: CERTIFICACIÓN, OPTIMIZACIÓN Y CIERRE (Post-Sprints)</t>
-  </si>
-  <si>
-    <t>T08</t>
-  </si>
-  <si>
-    <t>Infra/Cert</t>
-  </si>
-  <si>
-    <t>Implementar logging centralizado para errores de Flask y consultas SQL.</t>
-  </si>
-  <si>
     <t>Los errores críticos se registran en un archivo/base de datos.</t>
   </si>
   <si>
@@ -340,6 +384,9 @@
     <t>T09</t>
   </si>
   <si>
+    <t>Persistencia</t>
+  </si>
+  <si>
     <t>Optimización de consultas SQL: Creación de índices en las Claves Foráneas de PRESTAMOS y MATERIALES.</t>
   </si>
   <si>
@@ -368,6 +415,9 @@
   </si>
   <si>
     <t>T12</t>
+  </si>
+  <si>
+    <t>Frontend</t>
   </si>
   <si>
     <t>Implementar una página de Error 404 y Error 500 personalizada para mejorar la experiencia del usuario.</t>
@@ -431,7 +481,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,6 +492,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA2C4C9"/>
+        <bgColor rgb="FFA2C4C9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0E0E3"/>
+        <bgColor rgb="FFD0E0E3"/>
       </patternFill>
     </fill>
     <fill>
@@ -511,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -530,19 +592,19 @@
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -554,6 +616,9 @@
     <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -563,8 +628,8 @@
     <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="11" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -575,8 +640,23 @@
     <xf borderId="0" fillId="12" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="12" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="13" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="13" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="14" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -896,16 +976,16 @@
       <c r="E3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="F3" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J3" s="5" t="s">
@@ -938,24 +1018,24 @@
         <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="G4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="F4" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J4" s="5" t="s">
@@ -988,28 +1068,28 @@
         <v>25</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="F5" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="H5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="F5" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>20</v>
@@ -1031,39 +1111,19 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="A6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1081,38 +1141,38 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="5">
-        <v>5.0</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="K7" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="F7" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1131,38 +1191,38 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="5">
-        <v>6.0</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>20</v>
+      <c r="K8" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1181,38 +1241,38 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="5">
-        <v>7.0</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="8">
+        <v>6.0</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="E9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>20</v>
+      <c r="K9" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -1231,19 +1291,39 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="8">
+        <v>7.0</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+      <c r="F10" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1261,38 +1341,38 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="10">
+      <c r="A11" s="8">
         <v>8.0</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="B11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="10">
-        <v>8.0</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="I11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="K11" s="10" t="s">
-        <v>49</v>
+      <c r="K11" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1311,38 +1391,38 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="10">
+      <c r="A12" s="8">
         <v>9.0</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="10" t="s">
+      <c r="F12" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="H12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="10">
-        <v>8.0</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>49</v>
+      <c r="K12" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1361,38 +1441,38 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="10">
+      <c r="A13" s="8">
         <v>10.0</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>27</v>
+      <c r="D13" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I13" s="10" t="s">
+      <c r="F13" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="I13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="K13" s="10" t="s">
-        <v>49</v>
+      <c r="K13" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -1411,39 +1491,19 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="10">
-        <v>13.0</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>49</v>
-      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1461,38 +1521,38 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="13">
+        <v>11.0</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="13">
+        <v>8.0</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -1511,19 +1571,39 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="13">
+        <v>12.0</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="13">
+        <v>8.0</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+      <c r="K16" s="13" t="s">
+        <v>61</v>
+      </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -1548,31 +1628,31 @@
         <v>65</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>66</v>
       </c>
       <c r="F17" s="13">
-        <v>13.0</v>
+        <v>5.0</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>35</v>
+        <v>57</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="J17" s="13" t="s">
         <v>67</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -1595,34 +1675,34 @@
         <v>14.0</v>
       </c>
       <c r="B18" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>57</v>
-      </c>
       <c r="D18" s="13" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>70</v>
       </c>
       <c r="F18" s="13">
-        <v>8.0</v>
+        <v>13.0</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>35</v>
+        <v>71</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -1645,34 +1725,34 @@
         <v>15.0</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>74</v>
       </c>
       <c r="F19" s="13">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>35</v>
+        <v>68</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="J19" s="13" t="s">
         <v>75</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1691,39 +1771,19 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="13">
-        <v>16.0</v>
-      </c>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F20" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="K20" s="13" t="s">
-        <v>68</v>
-      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -1741,38 +1801,38 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21">
-      <c r="A21" s="13">
-        <v>17.0</v>
-      </c>
-      <c r="B21" s="13" t="s">
+      <c r="A21" s="17">
+        <v>16.0</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="17">
+        <v>13.0</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="13" t="s">
+      <c r="K21" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="F21" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="K21" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -1791,19 +1851,39 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="17">
+        <v>17.0</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
+      <c r="F22" s="17">
+        <v>8.0</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>80</v>
+      </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1821,38 +1901,38 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23">
-      <c r="A23" s="16">
+      <c r="A23" s="17">
         <v>18.0</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="16" t="s">
+      <c r="B23" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="16">
+      <c r="C23" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="17">
         <v>8.0</v>
       </c>
-      <c r="G23" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K23" s="16" t="s">
-        <v>86</v>
+      <c r="G23" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -1871,38 +1951,38 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="16">
+      <c r="A24" s="17">
         <v>19.0</v>
       </c>
-      <c r="B24" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="16" t="s">
+      <c r="B24" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="G24" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="F24" s="16">
-        <v>13.0</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="K24" s="16" t="s">
-        <v>86</v>
+      <c r="H24" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="K24" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -1921,38 +2001,38 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25">
-      <c r="A25" s="16">
+      <c r="A25" s="17">
         <v>20.0</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>41</v>
+      <c r="B25" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="D25" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="G25" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="F25" s="16">
-        <v>8.0</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="K25" s="16" t="s">
-        <v>86</v>
+      <c r="H25" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="K25" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -1971,39 +2051,19 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26">
-      <c r="A26" s="16">
-        <v>21.0</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="16" t="s">
+      <c r="A26" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F26" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="I26" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="K26" s="16" t="s">
-        <v>86</v>
-      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -2021,38 +2081,38 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27">
-      <c r="A27" s="16">
-        <v>22.0</v>
-      </c>
-      <c r="B27" s="16" t="s">
+      <c r="A27" s="21">
+        <v>21.0</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="16" t="s">
+      <c r="F27" s="21">
+        <v>8.0</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H27" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I27" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="16">
-        <v>5.0</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="I27" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="J27" s="16" t="s">
+      <c r="K27" s="21" t="s">
         <v>98</v>
-      </c>
-      <c r="K27" s="16" t="s">
-        <v>86</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
@@ -2071,38 +2131,38 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28">
-      <c r="A28" s="16">
-        <v>23.0</v>
-      </c>
-      <c r="B28" s="16" t="s">
+      <c r="A28" s="21">
+        <v>22.0</v>
+      </c>
+      <c r="B28" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="16" t="s">
+      <c r="C28" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="F28" s="16">
-        <v>8.0</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="I28" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="J28" s="16" t="s">
+      <c r="F28" s="21">
+        <v>13.0</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="I28" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="K28" s="16" t="s">
-        <v>86</v>
+      <c r="K28" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
@@ -2121,19 +2181,39 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="21">
+        <v>23.0</v>
+      </c>
+      <c r="B29" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
+      <c r="C29" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" s="21">
+        <v>8.0</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="I29" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="K29" s="21" t="s">
+        <v>98</v>
+      </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -2151,38 +2231,38 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30">
-      <c r="A30" s="20">
+      <c r="A30" s="21">
         <v>24.0</v>
       </c>
-      <c r="B30" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="20" t="s">
+      <c r="B30" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="F30" s="20">
-        <v>5.0</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="I30" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J30" s="20" t="s">
+      <c r="C30" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="K30" s="20" t="s">
+      <c r="F30" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="G30" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="I30" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="21" t="s">
         <v>107</v>
+      </c>
+      <c r="K30" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
@@ -2201,38 +2281,38 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31">
-      <c r="A31" s="20">
+      <c r="A31" s="21">
         <v>25.0</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="20" t="s">
+      <c r="C31" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="20">
-        <v>8.0</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="H31" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="I31" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J31" s="20" t="s">
+      <c r="F31" s="21">
+        <v>5.0</v>
+      </c>
+      <c r="G31" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="I31" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="K31" s="20" t="s">
-        <v>107</v>
+      <c r="K31" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
@@ -2251,38 +2331,38 @@
       <c r="Z31" s="2"/>
     </row>
     <row r="32">
-      <c r="A32" s="20">
+      <c r="A32" s="21">
         <v>26.0</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="C32" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="20" t="s">
+      <c r="C32" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="F32" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="H32" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="I32" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J32" s="20" t="s">
+      <c r="F32" s="21">
+        <v>8.0</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="I32" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="K32" s="20" t="s">
-        <v>107</v>
+      <c r="K32" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
@@ -2301,39 +2381,19 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33">
-      <c r="A33" s="20">
-        <v>27.0</v>
-      </c>
-      <c r="B33" s="20" t="s">
+      <c r="A33" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="C33" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="F33" s="20">
-        <v>8.0</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="H33" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="I33" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J33" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="K33" s="20" t="s">
-        <v>107</v>
-      </c>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -2351,38 +2411,38 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34">
-      <c r="A34" s="20">
-        <v>28.0</v>
-      </c>
-      <c r="B34" s="20" t="s">
+      <c r="A34" s="26">
+        <v>27.0</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="F34" s="26">
+        <v>5.0</v>
+      </c>
+      <c r="G34" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="20" t="s">
+      <c r="H34" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="I34" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="F34" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="I34" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="J34" s="20" t="s">
+      <c r="J34" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="K34" s="20" t="s">
-        <v>107</v>
+      <c r="K34" s="26" t="s">
+        <v>121</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
@@ -2401,38 +2461,38 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35">
-      <c r="A35" s="20">
-        <v>29.0</v>
-      </c>
-      <c r="B35" s="20" t="s">
+      <c r="A35" s="26">
+        <v>28.0</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F35" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="I35" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="J35" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="K35" s="26" t="s">
         <v>121</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="F35" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="I35" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J35" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="K35" s="20" t="s">
-        <v>107</v>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
@@ -2451,38 +2511,38 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36">
-      <c r="A36" s="20">
-        <v>30.0</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="D36" s="20" t="s">
+      <c r="A36" s="26">
+        <v>29.0</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E36" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="F36" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="I36" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J36" s="20" t="s">
+      <c r="E36" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="K36" s="20" t="s">
-        <v>107</v>
+      <c r="F36" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="G36" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H36" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="J36" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="K36" s="26" t="s">
+        <v>121</v>
       </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
@@ -2501,17 +2561,39 @@
       <c r="Z36" s="2"/>
     </row>
     <row r="37">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
+      <c r="A37" s="26">
+        <v>30.0</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F37" s="26">
+        <v>8.0</v>
+      </c>
+      <c r="G37" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H37" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="I37" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="J37" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="K37" s="26" t="s">
+        <v>121</v>
+      </c>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -2529,17 +2611,39 @@
       <c r="Z37" s="2"/>
     </row>
     <row r="38">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
+      <c r="A38" s="26">
+        <v>31.0</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="F38" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H38" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="I38" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="J38" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="K38" s="26" t="s">
+        <v>121</v>
+      </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -2557,17 +2661,39 @@
       <c r="Z38" s="2"/>
     </row>
     <row r="39">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
+      <c r="A39" s="26">
+        <v>32.0</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="F39" s="26">
+        <v>5.0</v>
+      </c>
+      <c r="G39" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H39" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="I39" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="J39" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="K39" s="26" t="s">
+        <v>121</v>
+      </c>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -2585,17 +2711,39 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
+      <c r="A40" s="26">
+        <v>33.0</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="F40" s="26">
+        <v>5.0</v>
+      </c>
+      <c r="G40" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="H40" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="I40" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="K40" s="26" t="s">
+        <v>121</v>
+      </c>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -4656,7 +4804,125 @@
       <c r="Y113" s="2"/>
       <c r="Z113" s="2"/>
     </row>
+    <row r="114">
+      <c r="A114" s="2"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2"/>
+      <c r="K114" s="2"/>
+      <c r="L114" s="2"/>
+      <c r="M114" s="2"/>
+      <c r="N114" s="2"/>
+      <c r="O114" s="2"/>
+      <c r="P114" s="2"/>
+      <c r="Q114" s="2"/>
+      <c r="R114" s="2"/>
+      <c r="S114" s="2"/>
+      <c r="T114" s="2"/>
+      <c r="U114" s="2"/>
+      <c r="V114" s="2"/>
+      <c r="W114" s="2"/>
+      <c r="X114" s="2"/>
+      <c r="Y114" s="2"/>
+      <c r="Z114" s="2"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="2"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
+      <c r="K115" s="2"/>
+      <c r="L115" s="2"/>
+      <c r="M115" s="2"/>
+      <c r="N115" s="2"/>
+      <c r="O115" s="2"/>
+      <c r="P115" s="2"/>
+      <c r="Q115" s="2"/>
+      <c r="R115" s="2"/>
+      <c r="S115" s="2"/>
+      <c r="T115" s="2"/>
+      <c r="U115" s="2"/>
+      <c r="V115" s="2"/>
+      <c r="W115" s="2"/>
+      <c r="X115" s="2"/>
+      <c r="Y115" s="2"/>
+      <c r="Z115" s="2"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="2"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+      <c r="J116" s="2"/>
+      <c r="K116" s="2"/>
+      <c r="L116" s="2"/>
+      <c r="M116" s="2"/>
+      <c r="N116" s="2"/>
+      <c r="O116" s="2"/>
+      <c r="P116" s="2"/>
+      <c r="Q116" s="2"/>
+      <c r="R116" s="2"/>
+      <c r="S116" s="2"/>
+      <c r="T116" s="2"/>
+      <c r="U116" s="2"/>
+      <c r="V116" s="2"/>
+      <c r="W116" s="2"/>
+      <c r="X116" s="2"/>
+      <c r="Y116" s="2"/>
+      <c r="Z116" s="2"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="2"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+      <c r="J117" s="2"/>
+      <c r="K117" s="2"/>
+      <c r="L117" s="2"/>
+      <c r="M117" s="2"/>
+      <c r="N117" s="2"/>
+      <c r="O117" s="2"/>
+      <c r="P117" s="2"/>
+      <c r="Q117" s="2"/>
+      <c r="R117" s="2"/>
+      <c r="S117" s="2"/>
+      <c r="T117" s="2"/>
+      <c r="U117" s="2"/>
+      <c r="V117" s="2"/>
+      <c r="W117" s="2"/>
+      <c r="X117" s="2"/>
+      <c r="Y117" s="2"/>
+      <c r="Z117" s="2"/>
+    </row>
   </sheetData>
+  <autoFilter ref="$A$1:$K$40"/>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I3:I5 I7:I13 I15:I19 I21:I25 I27:I32 I34:I40">
+      <formula1>"DONE,TO DO"</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>